<commit_message>
changes to base-sheet of stock comparator
</commit_message>
<xml_diff>
--- a/assets/base-sheet.xlsx
+++ b/assets/base-sheet.xlsx
@@ -478,7 +478,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -637,10 +637,6 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -860,8 +856,8 @@
   </sheetPr>
   <dimension ref="A1:T1009"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G37" activeCellId="0" sqref="G37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E48" activeCellId="0" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1612,9 +1608,18 @@
         <f aca="false">B13</f>
         <v>PCF</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="34"/>
+      <c r="C28" s="33" t="n">
+        <f aca="false">C13</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="33" t="n">
+        <f aca="false">D13</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="33" t="n">
+        <f aca="false">E13</f>
+        <v>0</v>
+      </c>
       <c r="G28" s="30"/>
       <c r="H28" s="30"/>
       <c r="I28" s="4"/>
@@ -1660,9 +1665,18 @@
         <f aca="false">"Valuacion " &amp; B29</f>
         <v>Valuacion PCF 5-Yr</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="34"/>
+      <c r="C30" s="33" t="e">
+        <f aca="false">(C$18*C29)/C28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D30" s="33" t="e">
+        <f aca="false">(D$18*D29)/D28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E30" s="33" t="e">
+        <f aca="false">(E$18*E29)/E28</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G30" s="30"/>
       <c r="H30" s="30"/>
       <c r="I30" s="4"/>
@@ -1834,7 +1848,7 @@
         <f aca="false">(C$18*C35)/C34</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D36" s="40" t="e">
+      <c r="D36" s="35" t="e">
         <f aca="false">(D$18*D35)/D34</f>
         <v>#DIV/0!</v>
       </c>
@@ -1882,15 +1896,15 @@
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
       <c r="B38" s="8"/>
-      <c r="C38" s="41" t="n">
+      <c r="C38" s="40" t="n">
         <f aca="false">C2</f>
         <v>0</v>
       </c>
-      <c r="D38" s="41" t="n">
+      <c r="D38" s="40" t="n">
         <f aca="false">D2</f>
         <v>0</v>
       </c>
-      <c r="E38" s="41" t="n">
+      <c r="E38" s="40" t="n">
         <f aca="false">E2</f>
         <v>0</v>
       </c>
@@ -1912,18 +1926,18 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="43" t="e">
+      <c r="C39" s="42" t="e">
         <f aca="false">AVERAGE(C27, C30, C33,C36)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D39" s="43" t="e">
+      <c r="D39" s="42" t="e">
         <f aca="false">AVERAGE(D27, D30, D33,D36)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E39" s="43" t="e">
+      <c r="E39" s="42" t="e">
         <f aca="false">AVERAGE(E27, E30, E33,E36)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1948,15 +1962,15 @@
       <c r="B40" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="44" t="e">
+      <c r="C40" s="43" t="e">
         <f aca="false">AVERAGE(C19:C22)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D40" s="44" t="e">
+      <c r="D40" s="43" t="e">
         <f aca="false">AVERAGE(D19:D22)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E40" s="44" t="e">
+      <c r="E40" s="43" t="e">
         <f aca="false">AVERAGE(E19:E22)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1978,18 +1992,18 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
-      <c r="B41" s="45" t="s">
+      <c r="B41" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="46" t="e">
+      <c r="C41" s="45" t="e">
         <f aca="false">AVERAGE(C39:C40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D41" s="46" t="e">
+      <c r="D41" s="45" t="e">
         <f aca="false">AVERAGE(D39:D40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E41" s="46" t="e">
+      <c r="E41" s="45" t="e">
         <f aca="false">AVERAGE(E39:E40)</f>
         <v>#DIV/0!</v>
       </c>
@@ -2033,19 +2047,19 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="48" t="e">
-        <f aca="false">(C22-C41)/C22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D43" s="48" t="e">
-        <f aca="false">(D22-D41)/D22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E43" s="48" t="e">
-        <f aca="false">(E22-E41)/E22</f>
+      <c r="C43" s="47" t="e">
+        <f aca="false">(C$18-C41)/C$18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D43" s="47" t="e">
+        <f aca="false">(D$18-D41)/D$18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E43" s="47" t="e">
+        <f aca="false">(E$18-E41)/E$18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F43" s="30"/>
@@ -2066,20 +2080,20 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
-      <c r="B44" s="47" t="str">
+      <c r="B44" s="46" t="str">
         <f aca="false">"Diff " &amp; B26 &amp; " %"</f>
         <v>Diff PER 5-Yr %</v>
       </c>
-      <c r="C44" s="48" t="e">
-        <f aca="false">(C19-C27)/C19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D44" s="48" t="e">
-        <f aca="false">(D19-D27)/D19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E44" s="48" t="e">
-        <f aca="false">(E19-E27)/E19</f>
+      <c r="C44" s="47" t="e">
+        <f aca="false">(C$18-C27)/C$18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D44" s="47" t="e">
+        <f aca="false">(D$18-D27)/D$18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E44" s="47" t="e">
+        <f aca="false">(E$18-E27)/E$18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F44" s="30"/>
@@ -2100,20 +2114,20 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
-      <c r="B45" s="47" t="str">
+      <c r="B45" s="46" t="str">
         <f aca="false">"Diff " &amp; B29 &amp; " %"</f>
         <v>Diff PCF 5-Yr %</v>
       </c>
-      <c r="C45" s="48" t="e">
-        <f aca="false">(C20-C230)/C20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D45" s="48" t="e">
-        <f aca="false">(D20-D230)/D20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E45" s="48" t="e">
-        <f aca="false">(E20-E230)/E20</f>
+      <c r="C45" s="47" t="e">
+        <f aca="false">(C$18-C30)/C$18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D45" s="47" t="e">
+        <f aca="false">(D$18-D30)/D$18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E45" s="47" t="e">
+        <f aca="false">(E$18-E30)/E$18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F45" s="4"/>
@@ -2134,20 +2148,20 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
-      <c r="B46" s="47" t="str">
+      <c r="B46" s="46" t="str">
         <f aca="false">"Diff " &amp; B32 &amp; " %"</f>
         <v>Diff PS 5-Yr %</v>
       </c>
-      <c r="C46" s="48" t="e">
-        <f aca="false">(C21-C33)/C21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D46" s="48" t="e">
-        <f aca="false">(D21-D33)/D21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E46" s="48" t="e">
-        <f aca="false">(E21-E33)/E21</f>
+      <c r="C46" s="47" t="e">
+        <f aca="false">(C$18-C33)/C$18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D46" s="47" t="e">
+        <f aca="false">(D$18-D33)/D$18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E46" s="47" t="e">
+        <f aca="false">(E$18-E33)/E$18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F46" s="4"/>
@@ -2168,20 +2182,20 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
-      <c r="B47" s="47" t="str">
+      <c r="B47" s="46" t="str">
         <f aca="false">"Diff " &amp; B35 &amp; " %"</f>
         <v>Diff PBV 5-Yr %</v>
       </c>
-      <c r="C47" s="48" t="e">
-        <f aca="false">(C22-C36)/C22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D47" s="48" t="e">
-        <f aca="false">(D22-D36)/D22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E47" s="48" t="e">
-        <f aca="false">(E22-E36)/E22</f>
+      <c r="C47" s="47" t="e">
+        <f aca="false">(C$18-C36)/C$18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D47" s="47" t="e">
+        <f aca="false">(D$18-D36)/D$18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E47" s="47" t="e">
+        <f aca="false">(E$18-E36)/E$18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F47" s="4"/>

</xml_diff>